<commit_message>
latest updates for schematic and layout
</commit_message>
<xml_diff>
--- a/Goose_6/TestRig/Control_Test_Board/Project Outputs for Control_Test_Board/BOM/Bill of Materials-Control_Test_Board.xlsx
+++ b/Goose_6/TestRig/Control_Test_Board/Project Outputs for Control_Test_Board/BOM/Bill of Materials-Control_Test_Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd57e3b774e874a1/Documents/GitHub/Motor-Control/Goose_6/TestRig/Control_Test_Board/Project Outputs for Control_Test_Board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{0D559A50-774C-4E6C-AB17-FA96D39AD8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43043DDD-9BBD-4251-856D-3480D36A09D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB03568F-8940-425D-A16F-E6DAD6F161A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{80487370-E940-44E2-B826-E1235B00B6B6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{17F3BC54-C18F-43F3-B93E-B12516FE8BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Control_Test_" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>Designator</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>535-13460-1-ND</t>
-  </si>
-  <si>
-    <t>Yageo</t>
   </si>
 </sst>
 </file>
@@ -634,23 +631,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9A38F5-3B4F-4E10-B7D5-F06D802EC981}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4480BB3D-576B-431C-B0C1-76C46EB0A7AC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18.26171875" customWidth="1"/>
-    <col min="2" max="5" width="15.3125" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" customWidth="1"/>
-    <col min="7" max="7" width="21.41796875" customWidth="1"/>
-    <col min="8" max="8" width="7.89453125" customWidth="1"/>
+    <col min="2" max="7" width="15.3125" customWidth="1"/>
+    <col min="8" max="8" width="18.26171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -690,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>

</xml_diff>